<commit_message>
remove tables and move objects further down
</commit_message>
<xml_diff>
--- a/category_data.xlsx
+++ b/category_data.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khuyenle/Desktop/SummerResearch.nosync/disCon/experiments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khuyenle/Desktop/SummerResearch.nosync/disCon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5D14A3B-B110-5246-B7AD-ACDA330EE983}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EF6A6642-61B1-FC4E-9619-61C276BA6116}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="18980" windowHeight="17440" xr2:uid="{BCA20CF7-FC44-9840-ADF4-04D1C5891860}"/>
+    <workbookView xWindow="14620" yWindow="1900" windowWidth="18980" windowHeight="17440" xr2:uid="{BCA20CF7-FC44-9840-ADF4-04D1C5891860}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="24 months" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Category</t>
   </si>
@@ -148,6 +148,84 @@
   </si>
   <si>
     <t>Normative sample</t>
+  </si>
+  <si>
+    <t>24 months</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Nail</t>
+  </si>
+  <si>
+    <t>Shovel</t>
+  </si>
+  <si>
+    <t>Broom</t>
+  </si>
+  <si>
+    <t>Hammer</t>
+  </si>
+  <si>
+    <t>Scissors</t>
+  </si>
+  <si>
+    <t>Sky object</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Moon</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>Furniture</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>Closet</t>
+  </si>
+  <si>
+    <t>Bed</t>
+  </si>
+  <si>
+    <t>Sofa</t>
+  </si>
+  <si>
+    <t>Lamp</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Fireman</t>
+  </si>
+  <si>
+    <t>Police</t>
+  </si>
+  <si>
+    <t>Mailman</t>
+  </si>
+  <si>
+    <t>Farmer (farm)</t>
   </si>
 </sst>
 </file>
@@ -514,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD572F0-C952-5C41-B27F-1FFF7AD62853}">
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,25 +619,22 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0.91</v>
+      <c r="C2" t="s">
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>0.81</v>
+        <v>0.91</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -567,69 +642,61 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>0.79</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>0.77</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>0.74</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>0.73</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>11</v>
-      </c>
-      <c r="C9">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>14</v>
       </c>
       <c r="C10">
         <v>0.87</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11">
-        <v>0.69</v>
+        <v>0.87</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -642,40 +709,40 @@
     </row>
     <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>0.63</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+        <v>0.69</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>0.54</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+        <v>0.63</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>0.31</v>
+        <v>0.54</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -686,31 +753,31 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>0.31</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>0.92</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17">
-        <v>0.82</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -723,10 +790,10 @@
     </row>
     <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C18">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -736,47 +803,46 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C20">
-        <v>0.74</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
+        <v>0.76</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C21">
-        <v>0.67</v>
-      </c>
-      <c r="D21" s="2"/>
+        <v>0.74</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -787,6 +853,13 @@
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>0.67</v>
+      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -797,15 +870,6 @@
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23">
-        <v>0.73</v>
-      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -816,11 +880,14 @@
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24">
-        <v>0.77</v>
+        <v>0.73</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -832,6 +899,12 @@
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25">
+        <v>0.77</v>
+      </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -843,23 +916,22 @@
     </row>
     <row r="26" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="E26" s="2"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
     </row>
     <row r="27" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="E28" s="2"/>
@@ -884,15 +956,7 @@
       <c r="M29" s="2"/>
     </row>
     <row r="30" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30">
-        <v>0.8</v>
-      </c>
+      <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -903,8 +967,11 @@
       <c r="M30" s="2"/>
     </row>
     <row r="31" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C31">
         <v>0.8</v>
@@ -920,10 +987,10 @@
     </row>
     <row r="32" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C32">
-        <v>0.64</v>
+        <v>0.8</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -936,10 +1003,10 @@
     </row>
     <row r="33" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C33">
-        <v>0.56999999999999995</v>
+        <v>0.64</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -952,10 +1019,10 @@
     </row>
     <row r="34" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C34">
-        <v>0.55000000000000004</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -968,10 +1035,10 @@
     </row>
     <row r="35" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C35">
-        <v>0.51</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -982,37 +1049,40 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="38" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="36" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36">
+        <v>0.51</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="39" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>26</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>36</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <v>0.79</v>
       </c>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39">
-        <v>0.64</v>
-      </c>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C40">
-        <v>0.42</v>
+        <v>0.64</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -1021,6 +1091,12 @@
       <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41">
+        <v>0.42</v>
+      </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -1056,18 +1132,211 @@
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="F46" s="2"/>
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>0.59</v>
+      </c>
+      <c r="D46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48">
+        <v>0.39</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C50">
+        <v>0.31</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+    </row>
+    <row r="52" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52">
+        <v>0.72</v>
+      </c>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57">
+        <v>0.8</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64">
+        <v>0.53</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>65</v>
+      </c>
+      <c r="C66">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69">
+        <v>0.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes for meeting with Mike
</commit_message>
<xml_diff>
--- a/category_data.xlsx
+++ b/category_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khuyenle/Desktop/SummerResearch.nosync/disCon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EF6A6642-61B1-FC4E-9619-61C276BA6116}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1A218F3A-6BDA-0E44-9EEC-59ECB908A3DA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14620" yWindow="1900" windowWidth="18980" windowHeight="17440" xr2:uid="{BCA20CF7-FC44-9840-ADF4-04D1C5891860}"/>
+    <workbookView xWindow="9580" yWindow="2620" windowWidth="23020" windowHeight="17440" xr2:uid="{BCA20CF7-FC44-9840-ADF4-04D1C5891860}"/>
   </bookViews>
   <sheets>
     <sheet name="24 months" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Category</t>
   </si>
@@ -226,6 +226,33 @@
   </si>
   <si>
     <t>Farmer (farm)</t>
+  </si>
+  <si>
+    <t>Drawer</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>Dress</t>
+  </si>
+  <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t>Sock</t>
+  </si>
+  <si>
+    <t>Shoe</t>
+  </si>
+  <si>
+    <t>Jacket</t>
+  </si>
+  <si>
+    <t>Jeans</t>
   </si>
 </sst>
 </file>
@@ -254,12 +281,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -274,10 +307,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD572F0-C952-5C41-B27F-1FFF7AD62853}">
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,7 +661,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -681,7 +715,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
@@ -770,7 +804,7 @@
       <c r="K15" s="2"/>
     </row>
     <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
@@ -967,7 +1001,7 @@
       <c r="M30" s="2"/>
     </row>
     <row r="31" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B31" t="s">
@@ -1227,7 +1261,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="A57" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B57" t="s">
@@ -1267,75 +1301,146 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C61">
-        <v>0.24</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C62">
         <v>0.24</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>60</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>61</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <v>0.53</v>
       </c>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
         <v>64</v>
       </c>
-      <c r="C65">
+      <c r="C66">
         <v>0.3</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
         <v>65</v>
       </c>
-      <c r="C66">
+      <c r="C67">
         <v>0.26</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
         <v>62</v>
-      </c>
-      <c r="C67">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>63</v>
       </c>
       <c r="C68">
         <v>0.21</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
         <v>66</v>
       </c>
-      <c r="C69">
+      <c r="C70">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72" t="s">
+        <v>73</v>
+      </c>
+      <c r="C72">
+        <v>0.93</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>72</v>
+      </c>
+      <c r="C73">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>70</v>
+      </c>
+      <c r="C75">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>74</v>
+      </c>
+      <c r="C76">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>69</v>
+      </c>
+      <c r="C77">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>75</v>
+      </c>
+      <c r="C78">
+        <v>0.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
images for all categories
</commit_message>
<xml_diff>
--- a/category_data.xlsx
+++ b/category_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khuyenle/Desktop/SummerResearch.nosync/disCon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ABFD38A5-C73E-E840-910E-666E25C9F174}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{21C2CFA0-8793-C846-9182-F5A04B2C3999}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9580" yWindow="1900" windowWidth="15800" windowHeight="17440" xr2:uid="{BCA20CF7-FC44-9840-ADF4-04D1C5891860}"/>
   </bookViews>
@@ -252,7 +252,7 @@
     <t>Jacket</t>
   </si>
   <si>
-    <t>Jeans</t>
+    <t>Coat</t>
   </si>
 </sst>
 </file>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD572F0-C952-5C41-B27F-1FFF7AD62853}">
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,18 +1394,18 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C77">
-        <v>0.56000000000000005</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C78">
-        <v>0.27</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>